<commit_message>
BC hoahong all: sai tên cột
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongNhanVien_All.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongNhanVien_All.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Dinh Phuong\Source\Workspaces\tfsbanhang24\banhang24vn\banhang24\Template\ExportExcel\Report\BaoCaoChietKhau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\BanHang24\Source\banhang24\banhang24\Template\ExportExcel\Report\BaoCaoChietKhau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>Hoa hồng tư vấn</t>
   </si>
   <si>
-    <t>Hoa hồng bán gói dịch vụ</t>
-  </si>
-  <si>
     <t>Tổng</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Hoa hồng thực hiện theo y/cầu</t>
+  </si>
+  <si>
+    <t>Theo doanh thu</t>
   </si>
 </sst>
 </file>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -675,27 +675,27 @@
         <v>1</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
       <c r="G4" s="23"/>
       <c r="H4" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="23"/>
       <c r="L4" s="21" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
       <c r="P4" s="23"/>
       <c r="Q4" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="7" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -705,43 +705,43 @@
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="O5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="18"/>
     </row>

</xml_diff>